<commit_message>
Added creation of 128x128 video tree
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,20 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Folder Size</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Images</t>
   </si>
   <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>24h</t>
-  </si>
-  <si>
     <t>bmp</t>
   </si>
   <si>
@@ -57,6 +48,51 @@
   </si>
   <si>
     <t>bmp (2048x2048)</t>
+  </si>
+  <si>
+    <t>bmp (128x128)</t>
+  </si>
+  <si>
+    <t>Videos</t>
+  </si>
+  <si>
+    <t>128 tree</t>
+  </si>
+  <si>
+    <t>256 tree</t>
+  </si>
+  <si>
+    <t>512 tree</t>
+  </si>
+  <si>
+    <t>1024 tree</t>
+  </si>
+  <si>
+    <t>2048 tree</t>
+  </si>
+  <si>
+    <t>4096 tree</t>
+  </si>
+  <si>
+    <t>Folder Size (MB)</t>
+  </si>
+  <si>
+    <t>2h25 (240)</t>
+  </si>
+  <si>
+    <t>Full tree</t>
+  </si>
+  <si>
+    <t>24h (2379)</t>
+  </si>
+  <si>
+    <t>Creation Time</t>
+  </si>
+  <si>
+    <t>Resize Image</t>
+  </si>
+  <si>
+    <t>Create Video</t>
   </si>
 </sst>
 </file>
@@ -92,8 +128,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,87 +445,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B39870-C2D0-4119-AF57-5ACF5BC180BC}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2">
-        <v>205</v>
+        <v>246</v>
       </c>
       <c r="D2">
         <f>2.38*1024</f>
         <v>2437.12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>176</v>
+        <v>212</v>
       </c>
       <c r="D3">
         <f>1.67*1024</f>
         <v>1710.08</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="1">
+        <v>8.0069444444444443E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <f>3.12*1024</f>
-        <v>3194.88</v>
+        <f>3.75*1024</f>
+        <v>3840</v>
       </c>
       <c r="D4">
         <f>37.1*1024</f>
         <v>37990.400000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C9">
+        <f>2.81*1024</f>
+        <v>2877.44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>10</v>
+      </c>
+      <c r="C10">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>5.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>21.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>91.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <f>1.42*1024</f>
+        <v>1454.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <f>1.9*1024</f>
+        <v>1945.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small changes, added new statistics
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Images</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Folder Size (MB)</t>
   </si>
   <si>
-    <t>2h25 (240)</t>
-  </si>
-  <si>
     <t>Full tree</t>
   </si>
   <si>
@@ -93,6 +90,18 @@
   </si>
   <si>
     <t>Create Video</t>
+  </si>
+  <si>
+    <t>Image Count</t>
+  </si>
+  <si>
+    <t>Image per Video</t>
+  </si>
+  <si>
+    <t>2h34</t>
+  </si>
+  <si>
+    <t>2h25</t>
   </si>
 </sst>
 </file>
@@ -116,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -124,13 +133,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B39870-C2D0-4119-AF57-5ACF5BC180BC}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,177 +477,278 @@
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
       <c r="M1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2">
+        <v>240</v>
+      </c>
+      <c r="D2" s="2">
+        <v>256</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="M2" s="2">
+        <v>240</v>
+      </c>
+      <c r="N2" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3">
+        <v>60</v>
+      </c>
+      <c r="D3" s="3">
+        <v>64</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="M3" s="3">
+        <v>60</v>
+      </c>
+      <c r="N3" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C4">
         <v>246</v>
       </c>
-      <c r="D2">
+      <c r="D4">
+        <v>263</v>
+      </c>
+      <c r="E4">
         <f>2.38*1024</f>
         <v>2437.12</v>
       </c>
-      <c r="L2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1.638888888888889E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C5">
         <v>212</v>
       </c>
-      <c r="D3">
+      <c r="D5">
+        <v>226</v>
+      </c>
+      <c r="E5">
         <f>1.67*1024</f>
         <v>1710.08</v>
       </c>
-      <c r="L3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="1">
+      <c r="L5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="1">
         <v>8.0069444444444443E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="N5" s="1">
+        <v>0.17056712962962964</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <f>3.75*1024</f>
         <v>3840</v>
       </c>
-      <c r="D4">
+      <c r="D6">
+        <f>4*1024</f>
+        <v>4096</v>
+      </c>
+      <c r="E6">
         <f>37.1*1024</f>
         <v>37990.400000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="C7">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="D7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="D8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C9">
         <v>180</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="D9">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="C10">
         <v>720</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="D10">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="C11">
         <f>2.81*1024</f>
         <v>2877.44</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D11">
+        <f>3*1024</f>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C10">
+      <c r="C12">
         <v>1.1100000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="D12">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C11">
+      <c r="C13">
         <v>5.05</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="D13">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C12">
+      <c r="C14">
         <v>21.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="D14">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
+      <c r="C15">
         <v>91.7</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="D15">
+        <v>93.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <v>376</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="D16">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <f>1.42*1024</f>
         <v>1454.08</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16">
+      <c r="D17">
+        <f>1.44*1024</f>
+        <v>1474.56</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
         <f>1.9*1024</f>
         <v>1945.6</v>
+      </c>
+      <c r="D18">
+        <f>1.93 *1024</f>
+        <v>1976.32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected video creation time
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -468,7 +468,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +590,7 @@
         <v>8.0069444444444443E-2</v>
       </c>
       <c r="N5" s="1">
-        <v>0.17056712962962964</v>
+        <v>7.4722222222222232E-2</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed example to use webgl 1.0, Changed texture to Luminance only, actualised statistic
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -80,9 +80,6 @@
     <t>Full tree</t>
   </si>
   <si>
-    <t>24h (2379)</t>
-  </si>
-  <si>
     <t>Creation Time</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>2h25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22h </t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,30 +486,30 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
         <v>25</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2">
@@ -518,17 +518,22 @@
       <c r="D2" s="2">
         <v>256</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2">
+        <v>2048</v>
+      </c>
       <c r="M2" s="2">
         <v>240</v>
       </c>
       <c r="N2" s="2">
         <v>256</v>
       </c>
+      <c r="O2">
+        <v>2048</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
@@ -537,11 +542,16 @@
       <c r="D3" s="3">
         <v>64</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3">
+        <v>64</v>
+      </c>
       <c r="M3" s="3">
         <v>60</v>
       </c>
       <c r="N3" s="3">
+        <v>64</v>
+      </c>
+      <c r="O3">
         <v>64</v>
       </c>
     </row>
@@ -563,7 +573,7 @@
         <v>2437.12</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N4" s="1">
         <v>1.638888888888889E-2</v>
@@ -584,13 +594,16 @@
         <v>1710.08</v>
       </c>
       <c r="L5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M5" s="1">
         <v>8.0069444444444443E-2</v>
       </c>
       <c r="N5" s="1">
         <v>7.4722222222222232E-2</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.77178240740740733</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -725,7 +738,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -738,7 +751,7 @@
         <v>1474.56</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -749,6 +762,10 @@
       <c r="D18">
         <f>1.93 *1024</f>
         <v>1976.32</v>
+      </c>
+      <c r="E18">
+        <f>16*1024</f>
+        <v>16384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added small documentation, actualised statistics
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
-  <si>
-    <t>Images</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>bmp</t>
   </si>
@@ -38,24 +35,6 @@
     <t>jp2</t>
   </si>
   <si>
-    <t>bmp (256x256)</t>
-  </si>
-  <si>
-    <t>bmp (512x512)</t>
-  </si>
-  <si>
-    <t>bmp (1024x1024)</t>
-  </si>
-  <si>
-    <t>bmp (2048x2048)</t>
-  </si>
-  <si>
-    <t>bmp (128x128)</t>
-  </si>
-  <si>
-    <t>Videos</t>
-  </si>
-  <si>
     <t>128 tree</t>
   </si>
   <si>
@@ -74,9 +53,6 @@
     <t>4096 tree</t>
   </si>
   <si>
-    <t>Folder Size (MB)</t>
-  </si>
-  <si>
     <t>Full tree</t>
   </si>
   <si>
@@ -102,6 +78,12 @@
   </si>
   <si>
     <t xml:space="preserve">22h </t>
+  </si>
+  <si>
+    <t>Videos size on disk (MB)</t>
+  </si>
+  <si>
+    <t>Images Size on disk (MB)</t>
   </si>
 </sst>
 </file>
@@ -465,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B39870-C2D0-4119-AF57-5ACF5BC180BC}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E22" sqref="C22:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,39 +459,34 @@
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>16</v>
-      </c>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="L1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2">
@@ -522,18 +499,15 @@
         <v>2048</v>
       </c>
       <c r="M2" s="2">
-        <v>240</v>
-      </c>
-      <c r="N2" s="2">
         <v>256</v>
       </c>
-      <c r="O2">
+      <c r="N2">
         <v>2048</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
@@ -542,228 +516,193 @@
       <c r="D3" s="3">
         <v>64</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>64</v>
       </c>
       <c r="M3" s="3">
-        <v>60</v>
-      </c>
-      <c r="N3" s="3">
         <v>64</v>
       </c>
-      <c r="O3">
+      <c r="N3">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>246</v>
-      </c>
-      <c r="D4">
-        <v>263</v>
-      </c>
-      <c r="E4">
-        <f>2.38*1024</f>
-        <v>2437.12</v>
-      </c>
-      <c r="L4" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="1">
-        <v>1.638888888888889E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>212</v>
+        <v>246</v>
       </c>
       <c r="D5">
-        <v>226</v>
+        <v>263</v>
       </c>
       <c r="E5">
-        <f>1.67*1024</f>
-        <v>1710.08</v>
+        <f>2.05*1024</f>
+        <v>2099.1999999999998</v>
       </c>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="M5" s="1">
-        <v>8.0069444444444443E-2</v>
-      </c>
-      <c r="N5" s="1">
-        <v>7.4722222222222232E-2</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0.77178240740740733</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.638888888888889E-2</v>
+      </c>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6">
+        <v>212</v>
+      </c>
+      <c r="D6">
+        <v>226</v>
+      </c>
+      <c r="E6">
+        <f>1.44*1024</f>
+        <v>1474.56</v>
+      </c>
+      <c r="L6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="1">
+        <v>7.4722222222222232E-2</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0.77178240740740733</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <f>3.75*1024</f>
         <v>3840</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <f>4*1024</f>
         <v>4096</v>
       </c>
-      <c r="E6">
-        <f>37.1*1024</f>
-        <v>37990.400000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="E7">
+        <f>32*1024</f>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D9">
+        <v>1.18</v>
+      </c>
+      <c r="E9">
+        <v>9.4600000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>5.05</v>
+      </c>
+      <c r="D10">
+        <v>5.3</v>
+      </c>
+      <c r="E10">
+        <v>44.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>21.1</v>
+      </c>
+      <c r="D11">
+        <v>21.8</v>
+      </c>
+      <c r="E11">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>91.7</v>
+      </c>
+      <c r="D12">
+        <v>93.9</v>
+      </c>
+      <c r="E12">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>376</v>
+      </c>
+      <c r="D13">
+        <v>382</v>
+      </c>
+      <c r="E13">
+        <f>3.06*1024</f>
+        <v>3133.44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
-        <v>11.2</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>45</v>
-      </c>
-      <c r="D8">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>180</v>
-      </c>
-      <c r="D9">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>720</v>
-      </c>
-      <c r="D10">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11">
-        <f>2.81*1024</f>
-        <v>2877.44</v>
-      </c>
-      <c r="D11">
-        <f>3*1024</f>
-        <v>3072</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="D12">
-        <v>1.18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>5.05</v>
-      </c>
-      <c r="D13">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>21.1</v>
-      </c>
-      <c r="D14">
-        <v>21.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15">
-        <v>91.7</v>
-      </c>
-      <c r="D15">
-        <v>93.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16">
-        <v>376</v>
-      </c>
-      <c r="D16">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17">
+      <c r="C14" s="3">
         <f>1.42*1024</f>
         <v>1454.08</v>
       </c>
-      <c r="D17">
+      <c r="D14" s="3">
         <f>1.44*1024</f>
         <v>1474.56</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18">
+      <c r="E14" s="3">
+        <f>12*1024</f>
+        <v>12288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
         <f>1.9*1024</f>
         <v>1945.6</v>
       </c>
-      <c r="D18">
+      <c r="D15">
         <f>1.93 *1024</f>
         <v>1976.32</v>
       </c>
-      <c r="E18">
+      <c r="E15">
         <f>16*1024</f>
         <v>16384</v>
       </c>

</xml_diff>

<commit_message>
Changed with new data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
@@ -581,16 +581,16 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.81640625" customWidth="1"/>
+    <col min="1" max="1" width="29.77734375" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7265625" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2" t="s">
@@ -612,7 +612,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -633,7 +633,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -654,14 +654,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -686,7 +686,7 @@
       </c>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -710,7 +710,7 @@
         <v>0.77178240740740733</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -727,7 +727,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -744,7 +744,7 @@
         <v>9.4600000000000009</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -758,7 +758,7 @@
         <v>44.8</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -772,7 +772,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -786,7 +786,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -801,7 +801,7 @@
         <v>3133.44</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
@@ -818,7 +818,7 @@
         <v>12288</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -844,19 +844,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -865,7 +865,7 @@
       </c>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -877,11 +877,11 @@
       </c>
       <c r="F3" s="6">
         <f>B12/B11*1024</f>
-        <v>0.19018727751122116</v>
+        <v>0.24433471416735708</v>
       </c>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -893,14 +893,14 @@
       </c>
       <c r="F4">
         <f>B11/B3</f>
-        <v>40.73770491803279</v>
+        <v>2.5367801597309794</v>
       </c>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -909,7 +909,7 @@
       </c>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -928,7 +928,7 @@
       </c>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -940,30 +940,30 @@
       </c>
       <c r="F8" s="8">
         <f>F7*F4</f>
-        <v>3199676222.95082</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+        <v>199247237.32660782</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="9">
         <f>F3/1024*F8</f>
-        <v>594275.10718789406</v>
+        <v>47542.008575031527</v>
       </c>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="B11">
-        <v>96915</v>
+        <v>6035</v>
       </c>
       <c r="E11" t="s">
         <v>32</v>
@@ -976,32 +976,32 @@
       </c>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="4">
-        <v>18</v>
+        <v>1.44</v>
       </c>
       <c r="E12" t="s">
         <v>31</v>
       </c>
       <c r="F12" s="9">
         <f>F9*F11</f>
-        <v>534847.59646910464</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>42787.807717528376</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1014,81 +1014,81 @@
       </c>
       <c r="F17" s="9">
         <f>F12*(1-B17)</f>
-        <v>250936.01518550477</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>20074.881214840385</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="4">
-        <v>13.3</v>
+        <v>1.07</v>
       </c>
       <c r="E20" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="9">
         <f>F12/B12*(B12-B20)</f>
-        <v>139654.65018915507</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>10994.089482976038</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="E22" t="s">
         <v>41</v>
       </c>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="E23" t="s">
         <v>31</v>
       </c>
       <c r="F23" s="9">
         <f>F20*(1-B17)</f>
-        <v>65522.181742881789</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5158.1292010353754</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E31" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E32" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E33" t="s">
         <v>48</v>
       </c>

</xml_diff>